<commit_message>
Updated UserName in userCreation data sheet
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_SPN_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_SPN_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\OneDrive - Cognizant\Documents\GlobalTestSuite Project\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestAutomation1\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="77" activeTab="80"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="22" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -8961,8 +8961,8 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8986,7 +8986,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>1275</v>
@@ -19098,7 +19098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>